<commit_message>
Made changes to organize better the inventory items in the new order tab when the vendor is selected
</commit_message>
<xml_diff>
--- a/Data/Purchase Orders/PO_19.xlsx
+++ b/Data/Purchase Orders/PO_19.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="16185" windowHeight="8663"/>
   </bookViews>
   <sheets>
-    <sheet name="Berry Man Purchase Order" sheetId="2" r:id="rId1"/>
+    <sheet name="Sysco Purchase Order" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -25,15 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
-  <si>
-    <t>Berry Man Purchase Order</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
+  <si>
+    <t>Sysco Purchase Order</t>
   </si>
   <si>
     <t>Contact</t>
   </si>
   <si>
-    <t>John Berryman</t>
+    <t>Miguel Penido</t>
   </si>
   <si>
     <t>Purchase Order #</t>
@@ -42,9 +42,6 @@
     <t>Phone:</t>
   </si>
   <si>
-    <t>(585) 259-0503</t>
-  </si>
-  <si>
     <t>Date:</t>
   </si>
   <si>
@@ -54,18 +51,57 @@
     <t>Purchased Unit</t>
   </si>
   <si>
+    <t>Dairy</t>
+  </si>
+  <si>
+    <t>Order Amt</t>
+  </si>
+  <si>
+    <t>Current Price</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>CASE 30lb</t>
+  </si>
+  <si>
+    <t>Butter</t>
+  </si>
+  <si>
+    <t>CASE 20lb</t>
+  </si>
+  <si>
+    <t>Cheddar</t>
+  </si>
+  <si>
+    <t>CASE 10lb</t>
+  </si>
+  <si>
+    <t>Feta</t>
+  </si>
+  <si>
+    <t>6 1/2 Gallon</t>
+  </si>
+  <si>
+    <t>Heavy Cream</t>
+  </si>
+  <si>
+    <t>Mozzarella</t>
+  </si>
+  <si>
+    <t>Pepper Jack</t>
+  </si>
+  <si>
+    <t>Sour Cream</t>
+  </si>
+  <si>
+    <t>Dairy Total:</t>
+  </si>
+  <si>
     <t>Dry Goods</t>
   </si>
   <si>
-    <t>Order Amt</t>
-  </si>
-  <si>
-    <t>Current Price</t>
-  </si>
-  <si>
-    <t>Extension</t>
-  </si>
-  <si>
     <t>6# CANS</t>
   </si>
   <si>
@@ -91,6 +127,9 @@
   </si>
   <si>
     <t>Produce Total:</t>
+  </si>
+  <si>
+    <t>Dairy Total</t>
   </si>
   <si>
     <t>Dry Goods Total</t>
@@ -126,12 +165,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF96A6DA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -308,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -337,6 +382,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -624,7 +674,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -665,188 +715,371 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
+      <c r="B4" s="2">
+        <v>7778889999</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="3">
-        <v>42733</v>
+        <v>42744</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="6" spans="1:6" ht="29.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="7">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>14</v>
-      </c>
       <c r="D7" s="8">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E7" s="9">
-        <v>43.22</v>
+        <v>76.989999999999995</v>
       </c>
       <c r="F7" s="10">
-        <v>864.4</v>
+        <v>153.97999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="11">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="5">
+        <v>3</v>
+      </c>
+      <c r="E8" s="6">
+        <v>43.65</v>
+      </c>
+      <c r="F8" s="12">
+        <v>130.94999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="11">
+        <v>2</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="5">
+        <v>5</v>
+      </c>
+      <c r="E9" s="6">
+        <v>28.98</v>
+      </c>
+      <c r="F9" s="12">
+        <v>144.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="11">
+        <v>6</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="5">
+        <v>4</v>
+      </c>
+      <c r="E10" s="6">
+        <v>41.5</v>
+      </c>
+      <c r="F10" s="12">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="11">
+        <v>6</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="5">
+        <v>2</v>
+      </c>
+      <c r="E11" s="6">
+        <v>66.760000000000005</v>
+      </c>
+      <c r="F11" s="12">
+        <v>133.52000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="11">
+        <v>4</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="5">
+        <v>2</v>
+      </c>
+      <c r="E12" s="6">
+        <v>43.78</v>
+      </c>
+      <c r="F12" s="12">
+        <v>87.56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="11">
+        <v>2</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="5">
+        <v>3</v>
+      </c>
+      <c r="E13" s="6">
+        <v>12.4</v>
+      </c>
+      <c r="F13" s="12">
+        <v>37.200000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="16">
+        <v>854.11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="29.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="7">
+        <v>6</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="8">
+        <v>20</v>
+      </c>
+      <c r="E16" s="9">
+        <v>53.22</v>
+      </c>
+      <c r="F16" s="10">
+        <v>1064.4000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="11">
         <v>1</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="5">
+      <c r="B17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="5">
         <v>20</v>
       </c>
-      <c r="E8" s="6">
-        <v>27.89</v>
-      </c>
-      <c r="F8" s="12">
-        <v>557.79999999999995</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="16">
+      <c r="E17" s="6">
+        <v>17.89</v>
+      </c>
+      <c r="F17" s="12">
+        <v>357.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="18"/>
+      <c r="F18" s="19">
         <v>1422.2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="29.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="17" t="s">
+    <row r="19" spans="1:6" ht="29.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="17" t="s">
+      <c r="C19" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="F19" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="7">
+    </row>
+    <row r="20" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="7">
         <v>1</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="8">
+      <c r="B20" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="8">
         <v>100</v>
       </c>
-      <c r="E11" s="9">
-        <v>4.29</v>
-      </c>
-      <c r="F11" s="10">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="19">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="14" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D14" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="10">
+      <c r="E20" s="9">
+        <v>5.29</v>
+      </c>
+      <c r="F20" s="10">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="21"/>
+      <c r="F21" s="22">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="23" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D23" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="25"/>
+      <c r="F23" s="10">
+        <v>854.11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D24" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="23"/>
+      <c r="F24" s="12">
         <v>1422.2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D15" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="20"/>
-      <c r="F15" s="12">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="26">
-        <v>1851.2</v>
-      </c>
-    </row>
-    <row r="17" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="25" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D25" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="23"/>
+      <c r="F25" s="12">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="28"/>
+      <c r="F26" s="29">
+        <v>2805.31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:E16"/>
+  <mergeCells count="13">
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="D26:E26"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="155" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>